<commit_message>
updates to feature engineering v1
</commit_message>
<xml_diff>
--- a/output/feature_ideas_v1.xlsx
+++ b/output/feature_ideas_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward Sims\Documents\ml_projects\nerdycat\nfl-big-data-bowl\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F839E7FB-BEE7-4F10-9923-AFCAF64298A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342BAD4A-DA94-42C4-B132-5B083477D047}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A745776-B911-4206-8911-3B0816B3A891}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>PlayId</t>
   </si>
@@ -54,69 +54,33 @@
     <t>IsOffenseWinning</t>
   </si>
   <si>
-    <t>Season</t>
-  </si>
-  <si>
     <t>Scale?</t>
   </si>
   <si>
     <t>Quarter</t>
   </si>
   <si>
-    <t>GameClock_sec</t>
-  </si>
-  <si>
-    <t>GameClock_minute</t>
-  </si>
-  <si>
     <t>Down</t>
   </si>
   <si>
     <t>Distance</t>
   </si>
   <si>
-    <t>RushingPosition</t>
-  </si>
-  <si>
     <t>[NE, KC, …]</t>
   </si>
   <si>
     <t>[RB, WR, TE, …]</t>
   </si>
   <si>
-    <t>InOwnTerritory</t>
-  </si>
-  <si>
     <t>OffenseFormation</t>
   </si>
   <si>
-    <t>[SHOTGUN, I_FORM, …]</t>
-  </si>
-  <si>
-    <t>NumberOfBacks</t>
-  </si>
-  <si>
-    <t>NumberOfWRs</t>
-  </si>
-  <si>
-    <t>NumberOfTEs</t>
-  </si>
-  <si>
     <t>Includes QB, RB, HB, FB</t>
   </si>
   <si>
-    <t>NumberOfDLinemen</t>
-  </si>
-  <si>
-    <t>NumberOfDBs</t>
-  </si>
-  <si>
     <t>Includes DE, DT, NT</t>
   </si>
   <si>
-    <t>NumberOfLBs</t>
-  </si>
-  <si>
     <t>Includes CB, FS, SS, S, SAF</t>
   </si>
   <si>
@@ -171,21 +135,12 @@
     <t>Week</t>
   </si>
   <si>
-    <t>Stadium</t>
-  </si>
-  <si>
-    <t>Might remove this…</t>
-  </si>
-  <si>
     <t>JerseyNumber</t>
   </si>
   <si>
     <t>Turf</t>
   </si>
   <si>
-    <t>[Grass, Artificial]</t>
-  </si>
-  <si>
     <t>GameWeather</t>
   </si>
   <si>
@@ -210,17 +165,101 @@
     <t>YardLine_std</t>
   </si>
   <si>
-    <t>To examine</t>
-  </si>
-  <si>
     <t>GameId</t>
+  </si>
+  <si>
+    <t>IsInEngland</t>
+  </si>
+  <si>
+    <t>StadiumType</t>
+  </si>
+  <si>
+    <t>[Grass, Artificial, Unknown]</t>
+  </si>
+  <si>
+    <t>Needs cleaning [Outdoor, Indoor, Unknown]</t>
+  </si>
+  <si>
+    <t>WindDirection</t>
+  </si>
+  <si>
+    <t>OffenseInOwnTerritory</t>
+  </si>
+  <si>
+    <t>NumberOfTEsOnPlay</t>
+  </si>
+  <si>
+    <t>NumberOfWRsOnPlay</t>
+  </si>
+  <si>
+    <t>NumberOfBacksOnPlay</t>
+  </si>
+  <si>
+    <t>NumberOfDBsOnPlay</t>
+  </si>
+  <si>
+    <t>NumberOfDLinemenOnPlay</t>
+  </si>
+  <si>
+    <t>NumberOfLBsOnPlay</t>
+  </si>
+  <si>
+    <t>NumberOfTeamRBsInGame</t>
+  </si>
+  <si>
+    <t>Feature Name</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Player Unique Features</t>
+  </si>
+  <si>
+    <t>More Complex Features (Play Unique)</t>
+  </si>
+  <si>
+    <t>Use PlayId and NflId. Does not have to have carried the ball</t>
+  </si>
+  <si>
+    <t>OffenseRushingPosition</t>
+  </si>
+  <si>
+    <t>Needs cleaning [0==East, 90==North….]</t>
+  </si>
+  <si>
+    <t>[SHOTGUN, I_FORM, …] Scaled to numbers</t>
+  </si>
+  <si>
+    <t>NumberOfOLinemenOnPlay</t>
+  </si>
+  <si>
+    <t>IsEvening</t>
+  </si>
+  <si>
+    <t>IsMorning</t>
+  </si>
+  <si>
+    <t>IsAfternoon</t>
+  </si>
+  <si>
+    <t>DayOfYear</t>
+  </si>
+  <si>
+    <t>MonthOfYear</t>
+  </si>
+  <si>
+    <t>QuarterGameSecs</t>
+  </si>
+  <si>
+    <t>TotalGameSecsPlayed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,13 +267,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -249,8 +301,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,280 +620,366 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19A3A37-5DA0-43E0-B55F-7B9F3DDB721C}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.77734375" customWidth="1"/>
-    <col min="3" max="6" width="8.33203125" customWidth="1"/>
+    <col min="3" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" s="1"/>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="E12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>55</v>
-      </c>
+      <c r="B34" s="1"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>57</v>
+      </c>
+      <c r="B50" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uploaded feature engineering and sub v1
</commit_message>
<xml_diff>
--- a/output/feature_ideas_v1.xlsx
+++ b/output/feature_ideas_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward Sims\Documents\ml_projects\nerdycat\nfl-big-data-bowl\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406B47D2-B038-4EE2-8DF8-E0A5043579C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E07D3D-B105-41D0-9D59-4E91759406B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A745776-B911-4206-8911-3B0816B3A891}"/>
   </bookViews>
@@ -255,9 +255,6 @@
     <t>Needs cleaning</t>
   </si>
   <si>
-    <t>IsStartingFirstHalf</t>
-  </si>
-  <si>
     <t>IsStartingScndHalf</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>(900 + QuarterGameSecs) where Quarter == 1 | 3</t>
+  </si>
+  <si>
+    <t>Removed could be unclear (turnovers on kick return/onside kicks)</t>
   </si>
 </sst>
 </file>
@@ -287,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +297,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,11 +319,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,16 +639,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19A3A37-5DA0-43E0-B55F-7B9F3DDB721C}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.77734375" customWidth="1"/>
+    <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8.33203125" customWidth="1"/>
@@ -901,10 +908,10 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -994,31 +1001,29 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="B46" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="A47" s="2"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
         <v>54</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B51" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>